<commit_message>
Add some more conditional formatted styles in the test workbooks #58130
git-svn-id: https://svn.apache.org/repos/asf/poi/trunk@1690530 13f79535-47bb-0310-9956-ffa450edef68
</commit_message>
<xml_diff>
--- a/test-data/spreadsheet/NewStyleConditionalFormattings.xlsx
+++ b/test-data/spreadsheet/NewStyleConditionalFormattings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Values</t>
   </si>
@@ -34,10 +34,46 @@
     <t>Colours BWR</t>
   </si>
   <si>
-    <t>Icon ??</t>
+    <t>Custom Icon+Format</t>
   </si>
   <si>
-    <t>Custom Icon+Format</t>
+    <t>Mixed icons</t>
+  </si>
+  <si>
+    <t>Icons - Default</t>
+  </si>
+  <si>
+    <t>Icons - 3 signs</t>
+  </si>
+  <si>
+    <t>Icons - 3 traffic lights 2</t>
+  </si>
+  <si>
+    <t>Icons - 4 traffic lights</t>
+  </si>
+  <si>
+    <t>Icons - 3 symbols</t>
+  </si>
+  <si>
+    <t>Icons - 3 flags</t>
+  </si>
+  <si>
+    <t>Icons - 3 symbols 2</t>
+  </si>
+  <si>
+    <t>Icons - 3 arrows</t>
+  </si>
+  <si>
+    <t>Icons - 5 arrows grey</t>
+  </si>
+  <si>
+    <t>Icons - 4 ratings</t>
+  </si>
+  <si>
+    <t>Icons - 5 ratings</t>
+  </si>
+  <si>
+    <t>Icons - 3 stars (ext)</t>
   </si>
 </sst>
 </file>
@@ -73,13 +109,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -94,634 +133,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1032,11 +443,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1045,68 +454,72 @@
     <col min="5" max="5" width="10.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.42578125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="20" max="20" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>6</v>
-      </c>
-      <c r="M1" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1115,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="D2">
-        <f t="shared" ref="D2:T17" si="0">$A2</f>
+        <f t="shared" ref="D2:U17" si="0">$A2</f>
         <v>1</v>
       </c>
       <c r="E2">
@@ -1182,8 +595,12 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
+      <c r="U2">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -1259,8 +676,12 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
+      <c r="U3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>15</v>
       </c>
@@ -1336,8 +757,12 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20</v>
       </c>
@@ -1413,8 +838,12 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>25</v>
       </c>
@@ -1490,8 +919,12 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>30</v>
       </c>
@@ -1567,8 +1000,12 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>34</v>
       </c>
@@ -1644,8 +1081,12 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>35</v>
       </c>
@@ -1721,8 +1162,12 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
+      <c r="U9">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>40</v>
       </c>
@@ -1798,8 +1243,12 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>50</v>
       </c>
@@ -1875,8 +1324,12 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
+      <c r="U11">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>25</v>
       </c>
@@ -1909,7 +1362,7 @@
         <v>25</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:T17" si="2">$A12</f>
+        <f t="shared" ref="J12:U17" si="2">$A12</f>
         <v>25</v>
       </c>
       <c r="K12">
@@ -1952,8 +1405,12 @@
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
+      <c r="U12">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0</v>
       </c>
@@ -1966,7 +1423,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <f t="shared" ref="E13:M17" si="3">$A13</f>
+        <f t="shared" ref="E13:I17" si="3">$A13</f>
         <v>0</v>
       </c>
       <c r="F13">
@@ -2029,8 +1486,12 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="U13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>-1</v>
       </c>
@@ -2106,8 +1567,12 @@
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
+      <c r="U14">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>-2</v>
       </c>
@@ -2183,8 +1648,12 @@
         <f t="shared" si="2"/>
         <v>-2</v>
       </c>
+      <c r="U15">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>-5</v>
       </c>
@@ -2260,8 +1729,12 @@
         <f t="shared" si="2"/>
         <v>-5</v>
       </c>
+      <c r="U16">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>-10</v>
       </c>
@@ -2337,21 +1810,25 @@
         <f t="shared" si="2"/>
         <v>-10</v>
       </c>
+      <c r="U17">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C17">
-    <cfRule type="cellIs" dxfId="5" priority="22" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="23" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D17">
-    <cfRule type="cellIs" dxfId="4" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="20" operator="between">
       <formula>10</formula>
       <formula>30</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17">
-    <cfRule type="dataBar" priority="18">
+    <cfRule type="dataBar" priority="19">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2365,7 +1842,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F17">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2377,7 +1854,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G17">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2389,7 +1866,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H17">
-    <cfRule type="iconSet" priority="15">
+    <cfRule type="iconSet" priority="16">
       <iconSet>
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -2398,7 +1875,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I17">
-    <cfRule type="iconSet" priority="14">
+    <cfRule type="iconSet" priority="15">
       <iconSet iconSet="3Signs">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -2407,7 +1884,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J17">
-    <cfRule type="iconSet" priority="13">
+    <cfRule type="iconSet" priority="14">
       <iconSet iconSet="3TrafficLights2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -2416,7 +1893,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K17">
-    <cfRule type="iconSet" priority="12">
+    <cfRule type="iconSet" priority="13">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -2426,7 +1903,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L17">
-    <cfRule type="iconSet" priority="11">
+    <cfRule type="iconSet" priority="12">
       <iconSet iconSet="3Symbols">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -2435,6 +1912,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2">
+    <cfRule type="iconSet" priority="11">
+      <iconSet iconSet="3Flags">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M17">
     <cfRule type="iconSet" priority="10">
       <iconSet iconSet="3Flags">
         <cfvo type="percent" val="0"/>
@@ -2443,17 +1929,8 @@
       </iconSet>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M2:M17">
+  <conditionalFormatting sqref="N2:N17">
     <cfRule type="iconSet" priority="9">
-      <iconSet iconSet="3Flags">
-        <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
-      </iconSet>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N2:N17">
-    <cfRule type="iconSet" priority="8">
       <iconSet iconSet="3Symbols2">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -2462,7 +1939,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O17">
-    <cfRule type="iconSet" priority="7">
+    <cfRule type="iconSet" priority="8">
       <iconSet iconSet="3Arrows">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -2471,7 +1948,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P17">
-    <cfRule type="iconSet" priority="6">
+    <cfRule type="iconSet" priority="7">
       <iconSet iconSet="5ArrowsGray">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -2482,7 +1959,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R17">
-    <cfRule type="iconSet" priority="4">
+    <cfRule type="iconSet" priority="5">
       <iconSet iconSet="4Rating">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -2492,7 +1969,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S17">
-    <cfRule type="iconSet" priority="3">
+    <cfRule type="iconSet" priority="4">
       <iconSet iconSet="5Rating">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="20"/>
@@ -2503,14 +1980,14 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T17">
-    <cfRule type="iconSet" priority="2">
+    <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3TrafficLights2">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="0"/>
         <cfvo type="formula" val="$T$5"/>
       </iconSet>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW($T2),2)=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2533,7 +2010,7 @@
           <xm:sqref>E2:E17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="5" id="{23404A22-2791-4FFE-B3BF-645D3DA783FE}">
+          <x14:cfRule type="iconSet" priority="6" id="{23404A22-2791-4FFE-B3BF-645D3DA783FE}">
             <x14:iconSet iconSet="3Stars">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -2548,6 +2025,25 @@
           </x14:cfRule>
           <xm:sqref>Q2:Q17</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{F6A45A70-DEA9-40B0-83E9-E53A5F349BE7}">
+            <x14:iconSet custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>30</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Signs" iconId="0"/>
+              <x14:cfIcon iconSet="3Flags" iconId="1"/>
+              <x14:cfIcon iconSet="3Symbols2" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>U2:U17</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>